<commit_message>
add row for BC LEEP row unit
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
+++ b/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="6135" windowWidth="19230" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
   <si>
     <t>m²</t>
   </si>
@@ -795,6 +795,9 @@
   </si>
   <si>
     <t>NZEH-Arch</t>
+  </si>
+  <si>
+    <t>BC-LEEP</t>
   </si>
 </sst>
 </file>
@@ -1717,18 +1720,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U9"/>
+  <dimension ref="B1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="47" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="47" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="47" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="47" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
@@ -1835,7 +1838,7 @@
         <v>11.5</v>
       </c>
       <c r="G3" s="66">
-        <f t="shared" ref="G3:G9" si="0">+E3/F3</f>
+        <f t="shared" ref="G3:G10" si="0">+E3/F3</f>
         <v>11.491304347826087</v>
       </c>
       <c r="H3" s="47">
@@ -1891,7 +1894,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="66">
-        <f>+C4/D4</f>
+        <f t="shared" ref="E4:E9" si="1">+C4/D4</f>
         <v>83.333333333333329</v>
       </c>
       <c r="F4" s="66">
@@ -1948,7 +1951,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="47">
-        <f>+C5/D5</f>
+        <f t="shared" si="1"/>
         <v>95.100000000000009</v>
       </c>
       <c r="F5" s="47">
@@ -2007,7 +2010,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="86">
-        <f>+C6/D6</f>
+        <f t="shared" si="1"/>
         <v>111.38429368029739</v>
       </c>
       <c r="F6" s="82">
@@ -2070,7 +2073,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="86">
-        <f>+C7/D7</f>
+        <f t="shared" si="1"/>
         <v>55.833333333333336</v>
       </c>
       <c r="F7" s="47">
@@ -2132,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="86">
-        <f>+C8/D8</f>
+        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
       <c r="F8" s="92">
@@ -2195,7 +2198,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="86">
-        <f>+C9/D9</f>
+        <f t="shared" si="1"/>
         <v>111.38429368029739</v>
       </c>
       <c r="F9" s="47">
@@ -2242,6 +2245,67 @@
       <c r="T9" s="88"/>
       <c r="U9" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="47">
+        <v>185.3</v>
+      </c>
+      <c r="D10" s="47">
+        <v>3</v>
+      </c>
+      <c r="E10" s="47">
+        <f>C10/D10</f>
+        <v>61.766666666666673</v>
+      </c>
+      <c r="F10" s="47">
+        <v>6.6040000000000001</v>
+      </c>
+      <c r="G10" s="47">
+        <f t="shared" si="0"/>
+        <v>9.3529174237835662</v>
+      </c>
+      <c r="H10" s="47">
+        <v>22</v>
+      </c>
+      <c r="I10" s="47">
+        <v>14</v>
+      </c>
+      <c r="J10" s="47">
+        <v>23</v>
+      </c>
+      <c r="K10" s="47">
+        <v>0</v>
+      </c>
+      <c r="L10" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="N10" s="88">
+        <v>2.72</v>
+      </c>
+      <c r="O10" s="88">
+        <v>3.02</v>
+      </c>
+      <c r="P10" s="88">
+        <v>2.77</v>
+      </c>
+      <c r="Q10" s="88">
+        <v>0</v>
+      </c>
+      <c r="R10" s="88">
+        <v>0</v>
+      </c>
+      <c r="S10" s="88">
+        <v>5.94</v>
+      </c>
+      <c r="T10" s="88">
+        <v>6.6040000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2259,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4275,14 +4339,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="N45:P45"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="N34:P34"/>
     <mergeCell ref="R34:T34"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="N45:P45"/>
   </mergeCells>
   <conditionalFormatting sqref="J34:L59">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
update archetype excel file based on comments from julia update heights of walls based on take-offs
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
+++ b/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
@@ -1723,7 +1723,7 @@
   <dimension ref="B1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,13 +2278,13 @@
         <v>23</v>
       </c>
       <c r="K10" s="47">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="L10" s="47">
         <v>0.5</v>
       </c>
       <c r="M10" s="47">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="N10" s="88">
         <v>2.72</v>
@@ -2324,7 +2324,7 @@
   <dimension ref="A2:T59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2347,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
@@ -2398,7 +2398,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="64">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,2,FALSE)</f>
-        <v>222.76858736059478</v>
+        <v>185.3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -2423,7 +2423,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="64">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,3,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" t="s">
@@ -2434,15 +2434,15 @@
       </c>
       <c r="I6" s="33">
         <f>+(INDEX(x1st,2)-INDEX(x1st,1))*(INDEX(z1st,7)-INDEX(z1st,2))</f>
-        <v>35.991000000000007</v>
+        <v>17.962880000000002</v>
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>31.475999999999996</v>
+        <v>19.94408</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
-        <v>0</v>
+        <v>18.293079999999996</v>
       </c>
       <c r="L6" t="s">
         <v>0</v>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="C7" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,4,FALSE)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>0</v>
@@ -2470,15 +2470,15 @@
       </c>
       <c r="I7" s="33">
         <f>+(INDEX(y1st,3)-INDEX(y1st,2))*(INDEX(z1st,7)-(INDEX(z1st,3)))</f>
-        <v>24.090091423878278</v>
+        <v>25.4399353926913</v>
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>21.068036944180278</v>
+        <v>28.245810619826369</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
-        <v>0</v>
+        <v>25.907581263880473</v>
       </c>
       <c r="L7" t="s">
         <v>0</v>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="C8" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,5,FALSE)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>1</v>
@@ -2506,15 +2506,15 @@
       </c>
       <c r="I8" s="33">
         <f>(INDEX(x1st,3)-INDEX(x1st,4))*(INDEX(z1st,7)-INDEX(z1st,4))</f>
-        <v>35.991000000000007</v>
+        <v>17.962880000000002</v>
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>31.475999999999996</v>
+        <v>19.94408</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
-        <v>0</v>
+        <v>18.293079999999996</v>
       </c>
       <c r="L8" t="s">
         <v>0</v>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="C9" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,6,FALSE)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>1</v>
@@ -2543,15 +2543,15 @@
       </c>
       <c r="I9" s="33">
         <f>(INDEX(y1st,4)-INDEX(y1st,1))*(INDEX(z1st,8)-INDEX(z1st,4))</f>
-        <v>24.090091423878278</v>
+        <v>25.4399353926913</v>
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>21.068036944180278</v>
+        <v>28.245810619826369</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
-        <v>0</v>
+        <v>25.907581263880473</v>
       </c>
       <c r="L9" t="s">
         <v>0</v>
@@ -2564,7 +2564,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,13,FALSE)</f>
-        <v>2.79</v>
+        <v>2.72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -2577,15 +2577,15 @@
       </c>
       <c r="I10" s="33">
         <f>INDEX(x1st,6)*INDEX(y1st,7)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="J10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="K10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
@@ -2598,7 +2598,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,14,FALSE)</f>
-        <v>2.44</v>
+        <v>3.02</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
@@ -2611,15 +2611,15 @@
       </c>
       <c r="I11" s="33">
         <f>INDEX(x1st,3)*INDEX(y1st,4)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="J11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="K11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="L11" t="s">
         <v>0</v>
@@ -2638,7 +2638,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,15,FALSE)</f>
-        <v>0</v>
+        <v>2.77</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
@@ -2651,34 +2651,34 @@
       </c>
       <c r="H12" s="43">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,7,FALSE)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I12" s="15">
         <f>AreaWall1*AreaWinWall1Ratio/100</f>
-        <v>6.4783800000000005</v>
+        <v>3.9518336000000005</v>
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>5.6656799999999983</v>
+        <v>4.3876976000000001</v>
       </c>
       <c r="K12" s="15">
         <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
-        <v>0</v>
+        <v>4.3876976000000001</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="27">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>4.6439999999999992</v>
+        <v>2.9057600000000003</v>
       </c>
       <c r="N12" s="26">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="O12">
         <f>+Len_WinWall1*Hght_WinWall1</f>
-        <v>6.4783800000000005</v>
+        <v>3.9518336000000009</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,16,FALSE)</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -2701,34 +2701,34 @@
       </c>
       <c r="H13" s="44">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,8,FALSE)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I13" s="17">
         <f>AreaWall2*AreaWinWall2Ratio/100</f>
-        <v>0</v>
+        <v>3.5615909549767819</v>
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>0</v>
+        <v>3.9544134867756919</v>
       </c>
       <c r="K13" s="17">
         <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
-        <v>0</v>
+        <v>3.9544134867756919</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M13" s="28">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>0</v>
+        <v>2.6188168786593984</v>
       </c>
       <c r="N13" s="29">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="O13">
         <f>+Len_WinWall2*Hght_WinWall2</f>
-        <v>0</v>
+        <v>3.5615909549767819</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,17,FALSE)</f>
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -2751,34 +2751,34 @@
       </c>
       <c r="H14" s="45">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,9,FALSE)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I14" s="18">
         <f>AreaWall3*AreaWinWall3Ratio/100</f>
-        <v>8.9977500000000017</v>
+        <v>4.1314624000000002</v>
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>7.8689999999999989</v>
+        <v>4.5871383999999997</v>
       </c>
       <c r="K14" s="18">
         <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
-        <v>0</v>
+        <v>4.5871383999999997</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="M14" s="30">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>6.45</v>
+        <v>3.0378400000000001</v>
       </c>
       <c r="N14" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="O14">
         <f>+Len_WinWall3*Hght_WinWall3</f>
-        <v>8.9977500000000017</v>
+        <v>4.1314624000000002</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2796,35 +2796,36 @@
       <c r="G15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="46">
-        <v>5</v>
+      <c r="H15" s="45">
+        <f>VLOOKUP($B$2,'Geometry options'!B4:O39,10,FALSE)</f>
+        <v>1E-3</v>
       </c>
       <c r="I15" s="20">
         <f>AreaWall4*AreaWinWall4Ratio/100</f>
-        <v>1.204504571193914</v>
+        <v>2.5439935392691299E-4</v>
       </c>
       <c r="J15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>1.0534018472090139</v>
+        <v>2.824581061982637E-4</v>
       </c>
       <c r="K15" s="20">
         <f>+IF(NumStoreys=3,AreaWall4_2nd*AreaWinWall4Ratio/100,0)</f>
-        <v>0</v>
+        <v>2.824581061982637E-4</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="M15" s="36">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>0.86344413705656897</v>
+        <v>1.8705834847567132E-4</v>
       </c>
       <c r="N15" s="32">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="O15">
         <f>+Len_WinWall4*Hght_WinWall4</f>
-        <v>1.204504571193914</v>
+        <v>2.5439935392691299E-4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2834,7 +2835,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="74">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,11,FALSE)</f>
-        <v>0.66700000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2853,7 +2854,7 @@
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
-        <v>11.970549999999999</v>
+        <v>10.161</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2875,7 +2876,7 @@
       </c>
       <c r="C18" s="11">
         <f>Opt_Width/2</f>
-        <v>6.45</v>
+        <v>3.302</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2888,7 +2889,7 @@
       </c>
       <c r="C19" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B3:U38,18,FALSE)</f>
-        <v>0</v>
+        <v>5.94</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -2901,7 +2902,7 @@
       </c>
       <c r="C20" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B4:U39,19,FALSE)</f>
-        <v>0</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -2914,7 +2915,7 @@
       </c>
       <c r="C21" s="11">
         <f>+C19*C20</f>
-        <v>0</v>
+        <v>39.227760000000004</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>0</v>
@@ -2940,7 +2941,7 @@
       </c>
       <c r="I23" s="42">
         <f>SUM(I6:I9)-SUM(I12:I15)</f>
-        <v>103.48154827656265</v>
+        <v>75.1604894310519</v>
       </c>
       <c r="J23" t="s">
         <v>0</v>
@@ -2952,7 +2953,7 @@
       </c>
       <c r="C24" s="15">
         <f>INDEX(x1st,10)</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="D24" s="1"/>
       <c r="F24" t="s">
@@ -2960,7 +2961,7 @@
       </c>
       <c r="I24" s="90">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
-        <v>90.499992041151543</v>
+        <v>83.450249294770856</v>
       </c>
       <c r="J24" t="s">
         <v>0</v>
@@ -2982,7 +2983,7 @@
       </c>
       <c r="I25" s="90">
         <f>+SUM(K6:K9)-SUM(K12:K15)</f>
-        <v>0</v>
+        <v>75.471790582879052</v>
       </c>
       <c r="J25" t="s">
         <v>0</v>
@@ -2995,14 +2996,14 @@
       </c>
       <c r="C26" s="17">
         <f>INDEX(y1st,14)</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="F26" t="s">
         <v>136</v>
       </c>
       <c r="I26">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>105.01916367597477</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
         <v>0</v>
@@ -3015,21 +3016,21 @@
       </c>
       <c r="C27" s="18">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="F27" t="s">
         <v>161</v>
       </c>
       <c r="I27">
         <f>+AreaWinWall1Ratio/100*SUM(I6:K6)+AreaWinWall2Ratio/100*SUM(I7:K7)+AreaWinWall3Ratio/100*SUM(I8:K8)+AreaWinWall4Ratio/100*SUM(I9:K9)</f>
-        <v>31.268716418402928</v>
+        <v>36.433879751968497</v>
       </c>
       <c r="J27" t="s">
         <v>0</v>
       </c>
       <c r="K27" s="90">
         <f>+SUM(I12:K15)</f>
-        <v>31.268716418402928</v>
+        <v>37.504205244094493</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3039,7 +3040,7 @@
       </c>
       <c r="C28" s="18">
         <f>INDEX(x1st,18)</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3048,7 +3049,7 @@
       </c>
       <c r="C29" s="19">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3057,7 +3058,7 @@
       </c>
       <c r="C30" s="20">
         <f>INDEX(y1st,22)</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -3153,7 +3154,7 @@
       </c>
       <c r="D36" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -3163,7 +3164,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -3173,7 +3174,7 @@
       </c>
       <c r="L36" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>0</v>
+        <v>5.74</v>
       </c>
       <c r="N36" s="24">
         <v>0</v>
@@ -3183,7 +3184,7 @@
       </c>
       <c r="P36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
       <c r="R36" s="24">
         <v>0</v>
@@ -3201,51 +3202,51 @@
       </c>
       <c r="B37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C37" s="24">
         <v>0</v>
       </c>
       <c r="D37" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G37" s="24">
         <v>0</v>
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K37" s="24">
         <v>0</v>
       </c>
       <c r="L37" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>0</v>
+        <v>5.74</v>
       </c>
       <c r="N37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="O37" s="24">
         <v>0</v>
       </c>
       <c r="P37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
       <c r="R37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="S37" s="24">
         <v>0</v>
@@ -3260,59 +3261,59 @@
       </c>
       <c r="B38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D38" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>0</v>
+        <v>5.74</v>
       </c>
       <c r="N38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="O38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
       <c r="R38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="S38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="T38" s="24">
         <v>0</v>
@@ -3327,51 +3328,51 @@
       </c>
       <c r="C39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D39" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
       <c r="G39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
       </c>
       <c r="K39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>0</v>
+        <v>5.74</v>
       </c>
       <c r="N39" s="24">
         <v>0</v>
       </c>
       <c r="O39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
       <c r="R39" s="24">
         <v>0</v>
       </c>
       <c r="S39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="T39" s="24">
         <v>0</v>
@@ -3389,7 +3390,7 @@
       </c>
       <c r="D40" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="F40" s="24">
         <v>0</v>
@@ -3399,7 +3400,7 @@
       </c>
       <c r="H40" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>5.74</v>
       </c>
       <c r="J40" s="24">
         <v>0</v>
@@ -3409,18 +3410,18 @@
       </c>
       <c r="L40" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>0</v>
+        <v>8.51</v>
       </c>
       <c r="N40" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.302</v>
       </c>
       <c r="O40" s="24">
         <v>0</v>
       </c>
       <c r="P40" s="24">
         <f>+C17</f>
-        <v>11.970549999999999</v>
+        <v>10.161</v>
       </c>
       <c r="R40" s="24">
         <v>0</v>
@@ -3430,7 +3431,7 @@
       </c>
       <c r="T40" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -3439,59 +3440,59 @@
       </c>
       <c r="B41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C41" s="24">
         <v>0</v>
       </c>
       <c r="D41" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="F41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G41" s="24">
         <v>0</v>
       </c>
       <c r="H41" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>5.74</v>
       </c>
       <c r="J41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K41" s="24">
         <v>0</v>
       </c>
       <c r="L41" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>0</v>
+        <v>8.51</v>
       </c>
       <c r="N41" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.302</v>
       </c>
       <c r="O41" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P41" s="24">
         <f>+C17</f>
-        <v>11.970549999999999</v>
+        <v>10.161</v>
       </c>
       <c r="R41" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="S41" s="24">
         <v>0</v>
       </c>
       <c r="T41" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -3500,53 +3501,53 @@
       </c>
       <c r="B42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D42" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="F42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H42" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>5.74</v>
       </c>
       <c r="J42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L42" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>0</v>
+        <v>8.51</v>
       </c>
       <c r="N42" s="83"/>
       <c r="O42" s="84"/>
       <c r="R42" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="S42" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="T42" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3558,33 +3559,33 @@
       </c>
       <c r="C43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D43" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>2.72</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
       </c>
       <c r="G43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H43" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>5.74</v>
       </c>
       <c r="J43" s="24">
         <v>0</v>
       </c>
       <c r="K43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L43" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>0</v>
+        <v>8.51</v>
       </c>
       <c r="N43" s="84"/>
       <c r="O43" s="84"/>
@@ -3593,11 +3594,11 @@
       </c>
       <c r="S43" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="T43" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>2.4384000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3614,7 +3615,7 @@
       </c>
       <c r="D44" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F44" s="26">
         <f>INDEX(x2nd,1)+0.5</f>
@@ -3626,7 +3627,7 @@
       </c>
       <c r="H44" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J44" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -3638,7 +3639,7 @@
       </c>
       <c r="L44" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -3647,7 +3648,7 @@
       </c>
       <c r="B45" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="C45" s="26">
         <f>INDEX(y1st,2)</f>
@@ -3655,11 +3656,11 @@
       </c>
       <c r="D45" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F45" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="G45" s="26">
         <f>INDEX(y2nd,2)</f>
@@ -3667,11 +3668,11 @@
       </c>
       <c r="H45" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J45" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="K45" s="26">
         <f>INDEX(y3rd,2)</f>
@@ -3679,7 +3680,7 @@
       </c>
       <c r="L45" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
       <c r="N45" s="96" t="s">
         <v>181</v>
@@ -3693,7 +3694,7 @@
       </c>
       <c r="B46" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="C46" s="26">
         <f>INDEX(y1st,5)</f>
@@ -3701,11 +3702,11 @@
       </c>
       <c r="D46" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F46" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="G46" s="26">
         <f>INDEX(y2nd,5)</f>
@@ -3713,11 +3714,11 @@
       </c>
       <c r="H46" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J46" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1439999999999992</v>
+        <v>3.4057600000000003</v>
       </c>
       <c r="K46" s="26">
         <f>INDEX(y3rd,5)</f>
@@ -3725,7 +3726,7 @@
       </c>
       <c r="L46" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="N46" s="91" t="s">
         <v>2</v>
@@ -3751,7 +3752,7 @@
       </c>
       <c r="D47" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F47" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -3763,7 +3764,7 @@
       </c>
       <c r="H47" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J47" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -3775,7 +3776,7 @@
       </c>
       <c r="L47" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="N47" s="24">
         <v>0</v>
@@ -3785,7 +3786,7 @@
       </c>
       <c r="P47" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3794,7 +3795,7 @@
       </c>
       <c r="B48" s="28">
         <f>INDEX(x1st,2)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C48" s="29">
         <f>INDEX(y1st,2)+0.5</f>
@@ -3802,11 +3803,11 @@
       </c>
       <c r="D48" s="29">
         <f>INDEX(z1st,2)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F48" s="28">
         <f>INDEX(x2nd,2)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G48" s="29">
         <f>INDEX(y2nd,2)+0.5</f>
@@ -3814,11 +3815,11 @@
       </c>
       <c r="H48" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J48" s="28">
         <f>INDEX(x3rd,2)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K48" s="29">
         <f>INDEX(y3rd,2)+0.5</f>
@@ -3826,18 +3827,18 @@
       </c>
       <c r="L48" s="29">
         <f>INDEX(z3rd,2)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
       <c r="N48" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="O48" s="24">
         <v>0</v>
       </c>
       <c r="P48" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3846,51 +3847,51 @@
       </c>
       <c r="B49" s="28">
         <f>INDEX(x1st,3)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C49" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="D49" s="29">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F49" s="28">
         <f>INDEX(x2nd,3)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G49" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="H49" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J49" s="28">
         <f>INDEX(x3rd,3)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K49" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="L49" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
       <c r="N49" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="O49" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P49" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3899,50 +3900,50 @@
       </c>
       <c r="B50" s="28">
         <f>INDEX(x1st,7)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C50" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="D50" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F50" s="28">
         <f>INDEX(x2nd,7)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G50" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="H50" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J50" s="28">
         <f>INDEX(x3rd,7)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K50" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.5</v>
+        <v>3.1188168786593984</v>
       </c>
       <c r="L50" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="N50" s="24">
         <v>0</v>
       </c>
       <c r="O50" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P50" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3951,7 +3952,7 @@
       </c>
       <c r="B51" s="28">
         <f>INDEX(x1st,6)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="C51" s="29">
         <f>INDEX(y1st,6)+0.5</f>
@@ -3959,11 +3960,11 @@
       </c>
       <c r="D51" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F51" s="28">
         <f>INDEX(x2nd,6)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="G51" s="29">
         <f>INDEX(y2nd,6)+0.5</f>
@@ -3971,11 +3972,11 @@
       </c>
       <c r="H51" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J51" s="28">
         <f>INDEX(x3rd,6)</f>
-        <v>12.9</v>
+        <v>6.6040000000000001</v>
       </c>
       <c r="K51" s="29">
         <f>INDEX(y3rd,6)+0.5</f>
@@ -3983,11 +3984,11 @@
       </c>
       <c r="L51" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="N51" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.302</v>
       </c>
       <c r="O51" s="24">
         <v>0</v>
@@ -4003,47 +4004,47 @@
       </c>
       <c r="B52" s="30">
         <f>INDEX(x1st,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="C52" s="31">
         <f>INDEX(y1st,3)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D52" s="31">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F52" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="G52" s="31">
         <f>INDEX(y2nd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H52" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J52" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="K52" s="31">
         <f>INDEX(y3rd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L52" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
       <c r="N52" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>3.302</v>
       </c>
       <c r="O52" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="P52" s="24">
         <f>+C32</f>
@@ -4056,39 +4057,39 @@
       </c>
       <c r="B53" s="30">
         <f>INDEX(x1st,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="C53" s="31">
         <f>INDEX(y1st,4)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D53" s="31">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F53" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="G53" s="31">
         <f>INDEX(y2nd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H53" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J53" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="K53" s="31">
         <f>INDEX(y3rd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L53" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4097,39 +4098,39 @@
       </c>
       <c r="B54" s="30">
         <f>INDEX(x1st,18)</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="C54" s="31">
         <f>INDEX(y1st,18)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D54" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F54" s="30">
         <f>INDEX(x2nd,18)</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="G54" s="31">
         <f>INDEX(y2nd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H54" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J54" s="30">
         <f>INDEX(x3rd,18)</f>
-        <v>5.95</v>
+        <v>3.06616</v>
       </c>
       <c r="K54" s="31">
         <f>INDEX(y3rd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L54" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4138,39 +4139,39 @@
       </c>
       <c r="B55" s="30">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="C55" s="31">
         <f>INDEX(y1st,19)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="D55" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F55" s="30">
         <f>INDEX(x2nd,17)</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="G55" s="31">
         <f>INDEX(y2nd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="H55" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J55" s="30">
         <f>INDEX(x3rd,17)</f>
-        <v>12.4</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="K55" s="31">
         <f>INDEX(y3rd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>9.3529174237835662</v>
       </c>
       <c r="L55" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4183,11 +4184,11 @@
       </c>
       <c r="C56" s="32">
         <f>INDEX(y1st,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="D56" s="32">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F56" s="32">
         <f>INDEX(x2nd,4)</f>
@@ -4195,11 +4196,11 @@
       </c>
       <c r="G56" s="32">
         <f>INDEX(y2nd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="H56" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J56" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -4207,11 +4208,11 @@
       </c>
       <c r="K56" s="32">
         <f>INDEX(y3rd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="L56" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4224,11 +4225,11 @@
       </c>
       <c r="C57" s="32">
         <f>INDEX(y1st,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="D57" s="32">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>2.9384000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F57" s="32">
         <f>INDEX(x2nd,1)</f>
@@ -4236,11 +4237,11 @@
       </c>
       <c r="G57" s="32">
         <f>INDEX(y2nd,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="H57" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>3.22</v>
       </c>
       <c r="J57" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -4248,11 +4249,11 @@
       </c>
       <c r="K57" s="32">
         <f>INDEX(y3rd,21)-Len_WinWall4</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="L57" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>0.5</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4265,11 +4266,11 @@
       </c>
       <c r="C58" s="32">
         <f>INDEX(y1st,22)</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="D58" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F58" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -4277,11 +4278,11 @@
       </c>
       <c r="G58" s="32">
         <f>INDEX(y2nd,22)</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="H58" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J58" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -4289,11 +4290,11 @@
       </c>
       <c r="K58" s="32">
         <f>INDEX(y3rd,22)</f>
-        <v>7.27099723350912</v>
+        <v>8.8527303654350913</v>
       </c>
       <c r="L58" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4306,11 +4307,11 @@
       </c>
       <c r="C59" s="32">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="D59" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>4.3334000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F59" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -4318,11 +4319,11 @@
       </c>
       <c r="G59" s="32">
         <f>INDEX(y2nd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="H59" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>7.1234000000000011</v>
+        <v>4.58</v>
       </c>
       <c r="J59" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -4330,23 +4331,23 @@
       </c>
       <c r="K59" s="32">
         <f>INDEX(y3rd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>8.8529174237835662</v>
       </c>
       <c r="L59" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>1.8950000000000002</v>
+        <v>7.6000000000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="R34:T34"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="J34:L34"/>
     <mergeCell ref="N45:P45"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="R34:T34"/>
   </mergeCells>
   <conditionalFormatting sqref="J34:L59">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -4471,15 +4472,15 @@
       </c>
       <c r="E7" s="55">
         <f>+main_area+second_area+third_area</f>
-        <v>193.98154031771418</v>
+        <v>234.08252930870179</v>
       </c>
       <c r="F7" s="55">
         <f>+E7*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>2519.640937225935</v>
       </c>
       <c r="G7" s="81">
         <f>+D7*F7</f>
-        <v>19924.139978755939</v>
+        <v>24042.973743218143</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -4528,15 +4529,15 @@
       </c>
       <c r="E10" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>234.08252930870179</v>
       </c>
       <c r="F10" s="55">
         <f>+E10*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>2519.640937225935</v>
       </c>
       <c r="G10" s="81">
         <f>+D10*F10</f>
-        <v>21835.818057760935</v>
+        <v>26349.845001300557</v>
       </c>
       <c r="H10" t="s">
         <v>144</v>
@@ -4585,15 +4586,15 @@
       </c>
       <c r="E13" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>234.08252930870179</v>
       </c>
       <c r="F13" s="55">
         <f>+E13*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>2519.640937225935</v>
       </c>
       <c r="G13" s="81">
         <f>+D13*F13</f>
-        <v>19856.860046363774</v>
+        <v>23961.785313018641</v>
       </c>
       <c r="H13" t="s">
         <v>172</v>
@@ -4642,15 +4643,15 @@
       </c>
       <c r="E16" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>234.08252930870179</v>
       </c>
       <c r="F16" s="55">
         <f>+E16*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>2519.640937225935</v>
       </c>
       <c r="G16" s="81">
         <f t="shared" ref="G16:G17" si="0">+D16*F16</f>
-        <v>31319.968527387653</v>
+        <v>37794.614058389023</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4666,15 +4667,15 @@
       </c>
       <c r="E17" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>193.98154031771418</v>
+        <v>234.08252930870179</v>
       </c>
       <c r="F17" s="55">
         <f>+E17*10.7639</f>
-        <v>2087.9979018258437</v>
+        <v>2519.640937225935</v>
       </c>
       <c r="G17" s="81">
         <f t="shared" si="0"/>
-        <v>33522.806313813919</v>
+        <v>40452.835247162388</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4727,15 +4728,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>0</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>0</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>4928.6127828883555</v>
+        <v>0</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -4782,15 +4783,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>0</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>0</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>10060.700405437243</v>
+        <v>0</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>
@@ -4818,15 +4819,15 @@
       </c>
       <c r="E26" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="F26" s="55">
         <f>+E26*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>664.85022333333336</v>
       </c>
       <c r="G26" s="68">
         <f>+F26*D26</f>
-        <v>1103.0150468457248</v>
+        <v>611.66220546666671</v>
       </c>
       <c r="H26" t="s">
         <v>170</v>
@@ -4845,15 +4846,15 @@
       </c>
       <c r="E27" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>61.766666666666673</v>
       </c>
       <c r="F27" s="55">
         <f>+E27*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>664.85022333333336</v>
       </c>
       <c r="G27" s="68">
         <f>+F27*D27</f>
-        <v>1198.929398745353</v>
+        <v>664.85022333333336</v>
       </c>
       <c r="H27" t="s">
         <v>171</v>
@@ -4980,15 +4981,15 @@
       </c>
       <c r="E37" s="47">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>36.433879751968497</v>
       </c>
       <c r="F37" s="55">
         <f t="shared" ref="F37:F40" si="1">+E37*10.7639</f>
-        <v>336.57333665604727</v>
+        <v>392.17063826221369</v>
       </c>
       <c r="G37" s="68">
         <f>+D37*F37</f>
-        <v>23760.981397166746</v>
+        <v>27685.96981818002</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -5004,15 +5005,15 @@
       </c>
       <c r="E38" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>36.433879751968497</v>
       </c>
       <c r="F38" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>392.17063826221369</v>
       </c>
       <c r="G38" s="68">
         <f t="shared" ref="G38:G40" si="2">+D38*F38</f>
-        <v>23760.981397166746</v>
+        <v>27685.96981818002</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -5028,15 +5029,15 @@
       </c>
       <c r="E39" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>36.433879751968497</v>
       </c>
       <c r="F39" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>392.17063826221369</v>
       </c>
       <c r="G39" s="68">
         <f t="shared" si="2"/>
-        <v>26538.405165588203</v>
+        <v>30922.185921357534</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -5052,15 +5053,15 @@
       </c>
       <c r="E40" s="89">
         <f>total_window_area</f>
-        <v>31.268716418402928</v>
+        <v>36.433879751968497</v>
       </c>
       <c r="F40" s="55">
         <f t="shared" si="1"/>
-        <v>336.57333665604727</v>
+        <v>392.17063826221369</v>
       </c>
       <c r="G40" s="68">
         <f t="shared" si="2"/>
-        <v>26538.405165588203</v>
+        <v>30922.185921357534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify basement wall height in archetype worksheet for BC-LEEP
update geometry files
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
+++ b/OptFramework/GenericHome-LEEP-BC/LEEP_BC_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6135" windowWidth="19230" windowHeight="5940"/>
+    <workbookView xWindow="-15" yWindow="6135" windowWidth="19230" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2296,7 @@
         <v>2.77</v>
       </c>
       <c r="Q10" s="88">
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="R10" s="88">
         <v>0</v>
@@ -2323,15 +2323,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>19.94408</v>
+        <v>19.944079999999996</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>28.245810619826369</v>
+        <v>28.245810619826365</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>19.94408</v>
+        <v>19.944079999999996</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>28.245810619826369</v>
+        <v>28.245810619826365</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2659,11 +2659,11 @@
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>4.3876976000000001</v>
+        <v>4.3876975999999992</v>
       </c>
       <c r="K12" s="15">
         <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
-        <v>4.3876976000000001</v>
+        <v>4.3876975999999992</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>0</v>
@@ -2688,7 +2688,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,16,FALSE)</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -2709,11 +2709,11 @@
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>3.9544134867756919</v>
+        <v>3.954413486775691</v>
       </c>
       <c r="K13" s="17">
         <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
-        <v>3.9544134867756919</v>
+        <v>3.954413486775691</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>0</v>
@@ -2759,11 +2759,11 @@
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>4.5871383999999997</v>
+        <v>4.5871383999999988</v>
       </c>
       <c r="K14" s="18">
         <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
-        <v>4.5871383999999997</v>
+        <v>4.5871383999999988</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="I24" s="90">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
-        <v>83.450249294770856</v>
+        <v>83.450249294770828</v>
       </c>
       <c r="J24" t="s">
         <v>0</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="I26">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="J26" t="s">
         <v>0</v>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="D36" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="L36" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N36" s="24">
         <v>0</v>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="P36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R36" s="24">
         <v>0</v>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="D37" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="L37" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N37" s="25">
         <f>Opt_Width</f>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="P37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R37" s="25">
         <f>Opt_Width</f>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D38" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N38" s="25">
         <f>Opt_Width</f>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="P38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R38" s="25">
         <f>Opt_Width</f>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="D39" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N39" s="24">
         <v>0</v>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="P39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R39" s="24">
         <v>0</v>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D40" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F40" s="24">
         <v>0</v>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="H40" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J40" s="24">
         <v>0</v>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="L40" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N40" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="P40" s="24">
         <f>+C17</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="R40" s="24">
         <v>0</v>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="T40" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="D41" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F41" s="25">
         <f>Opt_Width</f>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="H41" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J41" s="25">
         <f>Opt_Width</f>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="L41" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N41" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="P41" s="24">
         <f>+C17</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="R41" s="25">
         <f>Opt_Width</f>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="T41" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D42" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F42" s="25">
         <f>Opt_Width</f>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="H42" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J42" s="25">
         <f>Opt_Width</f>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="L42" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N42" s="83"/>
       <c r="O42" s="84"/>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="T42" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D43" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="H43" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J43" s="24">
         <v>0</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="L43" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N43" s="84"/>
       <c r="O43" s="84"/>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="T43" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3615,7 +3615,7 @@
       </c>
       <c r="D44" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F44" s="26">
         <f>INDEX(x2nd,1)+0.5</f>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="H44" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J44" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="L44" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="D45" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F45" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
@@ -3668,7 +3668,7 @@
       </c>
       <c r="H45" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J45" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="L45" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N45" s="96" t="s">
         <v>181</v>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="D46" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F46" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="H46" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J46" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="L46" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N46" s="91" t="s">
         <v>2</v>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="D47" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F47" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -3764,7 +3764,7 @@
       </c>
       <c r="H47" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J47" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="L47" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N47" s="24">
         <v>0</v>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="P47" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="D48" s="29">
         <f>INDEX(z1st,2)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F48" s="28">
         <f>INDEX(x2nd,2)</f>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="H48" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J48" s="28">
         <f>INDEX(x3rd,2)</f>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="L48" s="29">
         <f>INDEX(z3rd,2)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N48" s="25">
         <f>Opt_Width</f>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="P48" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="D49" s="29">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F49" s="28">
         <f>INDEX(x2nd,3)</f>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="H49" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J49" s="28">
         <f>INDEX(x3rd,3)</f>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="L49" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N49" s="25">
         <f>Opt_Width</f>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="P49" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="D50" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F50" s="28">
         <f>INDEX(x2nd,7)</f>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="H50" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J50" s="28">
         <f>INDEX(x3rd,7)</f>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="L50" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N50" s="24">
         <v>0</v>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="P50" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="D51" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F51" s="28">
         <f>INDEX(x2nd,6)</f>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="H51" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J51" s="28">
         <f>INDEX(x3rd,6)</f>
@@ -3984,7 +3984,7 @@
       </c>
       <c r="L51" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N51" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="D52" s="31">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F52" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="H52" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J52" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="L52" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N52" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="D53" s="31">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F53" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H53" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J53" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="L53" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D54" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F54" s="30">
         <f>INDEX(x2nd,18)</f>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="H54" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J54" s="30">
         <f>INDEX(x3rd,18)</f>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="L54" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D55" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F55" s="30">
         <f>INDEX(x2nd,17)</f>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="H55" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J55" s="30">
         <f>INDEX(x3rd,17)</f>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="L55" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D56" s="32">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F56" s="32">
         <f>INDEX(x2nd,4)</f>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="H56" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J56" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="L56" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="D57" s="32">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F57" s="32">
         <f>INDEX(x2nd,1)</f>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="H57" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J57" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="L57" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D58" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F58" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="H58" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J58" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="L58" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D59" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F59" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="H59" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J59" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="L59" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4728,15 +4728,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>0</v>
+        <v>837.63264995131067</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>0</v>
+        <v>3652.0783537877141</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -4783,15 +4783,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>0</v>
+        <v>837.63264995131067</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>0</v>
+        <v>7454.9305845666668</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>

</xml_diff>